<commit_message>
Wristband modification to fix timing conflicts in transmission
</commit_message>
<xml_diff>
--- a/Global_Localization/benchmarks/DecawaveBenchmarking.xlsx
+++ b/Global_Localization/benchmarks/DecawaveBenchmarking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -258,9 +258,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -268,6 +265,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -284,6 +284,1411 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Decawave Distance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Benchmarking</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-13-2017 (Dry)'!$CB$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Measured</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'4-13-2017 (Dry)'!$CB$4:$CB$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>0.1605027</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56302810000000025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86715380000000053</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2354858999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5715044000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9355247999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2740231000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6168448000000013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9343791999999986</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2794042000000023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5870898000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.9214675000000017</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.1580493999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.445052200000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.8630561000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0167105999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4481773999999987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.6865420000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.0823584999999989</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.2990560999999969</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.5211920000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.9763429999999991</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.3272755999999983</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.5903126999999992</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.0535768999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.2060144999999984</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.3144074999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.7779573999999965</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.0897225000000006</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.1000897000000016</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.8834716999999959</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10.143833199999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10.426193200000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.062065</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.227682600000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11.319565199999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11.705488800000003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11.862520999999994</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12.124383599999996</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.528926199999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12.679629500000006</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13.728627300000005</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14.214222200000009</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>14.442734500000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>14.269894300000006</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14.446253000000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14.5774422</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>15.031888900000006</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>15.602471899999996</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15.401396499999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>15.962268700000006</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>16.046319799999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>16.394674700000007</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>16.720746300000002</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>16.960564500000004</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>17.503004699999991</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>17.743995000000005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>18.002152900000002</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>18.1588566</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>18.448626199999989</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>19.467795100000004</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>19.897852100000005</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>19.919242499999992</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>20.600188799999991</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>20.922228299999997</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>21.137328700000012</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>21.414012599999996</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>21.681081199999998</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>21.917241700000005</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>22.194019400000013</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>22.692790800000008</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>23.012813799999989</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>23.496485399999997</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>23.437807599999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>23.506287599999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-63E7-4943-BFE9-764CD58F4193}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-13-2017 (Dry)'!$CC$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'4-13-2017 (Dry)'!$CC$4:$CC$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>0.3048780487804878</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6097560975609756</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91463414634146345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2195121951219512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.524390243902439</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8292682926829269</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1341463414634148</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4390243902439024</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7439024390243905</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0487804878048781</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3536585365853662</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6585365853658538</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.9634146341463419</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2682926829268295</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.5731707317073171</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8780487804878048</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.1829268292682933</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4878048780487809</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.7926829268292686</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.0975609756097562</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.4024390243902447</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.7073170731707323</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.01219512195122</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.3170731707317076</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.6219512195121952</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.9268292682926838</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.2317073170731714</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.536585365853659</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.8414634146341466</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.1463414634146343</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.4512195121951219</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.7560975609756095</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10.060975609756099</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10.365853658536587</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10.670731707317074</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10.975609756097562</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11.280487804878049</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11.585365853658537</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11.890243902439025</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.195121951219512</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12.804878048780489</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>13.109756097560977</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>13.414634146341465</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>13.719512195121952</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14.02439024390244</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14.329268292682928</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>14.634146341463415</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>14.939024390243903</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15.24390243902439</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>15.548780487804878</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>15.853658536585368</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>16.158536585365855</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>16.463414634146343</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>16.76829268292683</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>17.073170731707318</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>17.378048780487806</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>17.682926829268293</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>17.987804878048781</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>18.292682926829269</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>18.597560975609756</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>18.902439024390244</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>19.207317073170731</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>19.512195121951219</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>19.81707317073171</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>20.121951219512198</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>20.426829268292686</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>20.731707317073173</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>21.036585365853661</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>21.341463414634148</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>21.646341463414636</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>21.951219512195124</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>22.256097560975611</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>22.560975609756099</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>22.865853658536587</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-63E7-4943-BFE9-764CD58F4193}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="373599752"/>
+        <c:axId val="373592536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="373599752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="373592536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="373592536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="373599752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>536574</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>85</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C710ABBE-FED4-48A4-BCF2-460A53E97199}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -585,7 +1990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AV113"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -599,60 +2004,60 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:48" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="R2" s="1" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Z2" s="1" t="s">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Z2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AH2" s="1" t="s">
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AH2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AP2" s="1" t="s">
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AP2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1"/>
-      <c r="AV2" s="1"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
     </row>
     <row r="3" spans="2:48" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -9432,8 +10837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:CH113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
-      <selection activeCell="CG2" sqref="CG2"/>
+    <sheetView tabSelected="1" topLeftCell="BO36" workbookViewId="0">
+      <selection activeCell="CB3" sqref="CB3:CC78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35594,6 +36999,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -35617,48 +37023,48 @@
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.99941765641299607</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.99883565195004553</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.9988197019767584</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.22828049257693761</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>75</v>
       </c>
     </row>
@@ -35668,156 +37074,156 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>3263.4102809008882</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>3263.4102809008882</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>62623.029767778869</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>7.6043226617369791E-109</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>73</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>3.8041747802553565</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>5.211198329116927E-2</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>74</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>3267.2144556811436</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>2.5235020868803915E-2</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>5.3186574832096926E-2</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>0.47446222939656446</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>0.63658658116377631</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>-8.0765669907491039E-2</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>0.13123571164509887</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>-8.0765669907491039E-2</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>0.13123571164509887</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>0.96246798574834413</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>3.8460883372226332E-3</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>250.24593856400315</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>7.6043226617369791E-109</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>0.95480274274634092</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>0.97013322875034735</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>0.95480274274634092</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>0.97013322875034735</v>
       </c>
     </row>

</xml_diff>